<commit_message>
rename SQLQueryRequest to SQLRequest, put the parameters totalRows in sqlQueryRequest, modified the logic generate with iteration from totalRows and fleksible setValue and confitiona | test generate update with realData DONE | saveDbIn Local and DB underProgress | 7/242024
</commit_message>
<xml_diff>
--- a/src/main/resources/tmp_data/test_update.xlsx
+++ b/src/main/resources/tmp_data/test_update.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\iseng\hand_ql\src\main\resources\tmp_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA79D7D0-1EB7-49B9-968C-D8A77434DA61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{308B81CA-1182-4AD3-88D7-6498C2010E2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{5FC23102-1508-404A-9358-4B2D6E2DBA2B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>status</t>
   </si>
@@ -49,6 +49,12 @@
   </si>
   <si>
     <t>DELETED</t>
+  </si>
+  <si>
+    <t>type_order</t>
+  </si>
+  <si>
+    <t>SALE</t>
   </si>
 </sst>
 </file>
@@ -400,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D54E37D7-9056-44F0-8950-6FC14375B17A}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -412,7 +418,7 @@
     <col min="3" max="3" width="27.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -422,8 +428,11 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -432,6 +441,23 @@
       </c>
       <c r="C2">
         <v>1209380</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>1212121</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>